<commit_message>
Change the profiles in HCIM Stoma to use the new reasonReference extension on nl-core-observation
</commit_message>
<xml_diff>
--- a/Mappings/Stoma - STU3.xlsx
+++ b/Mappings/Stoma - STU3.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nicitz-stu3-zibs2017\Profiles-Staging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C054A49-401C-4941-B3D5-ACB310727C38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stoma 2017" sheetId="1" r:id="rId1"/>
     <sheet name="Valuesets 2017" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -361,16 +362,16 @@
     <t>Rechts en links</t>
   </si>
   <si>
-    <t>Observation.extension:MedicalDevice</t>
-  </si>
-  <si>
     <t>Observation.valueCoadeableConcept</t>
+  </si>
+  <si>
+    <t>(MedicalDevice.reasonReference can be used to refer to this Observation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -588,8 +589,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -934,11 +935,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1062,7 +1063,7 @@
         <v>24</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q4" s="10"/>
     </row>
@@ -1097,7 +1098,7 @@
         <v>32</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q5" s="10"/>
     </row>
@@ -1252,10 +1253,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O4" location="StomaTypeCodelist!A1" display="StomaTypeCodelist"/>
-    <hyperlink ref="O5" r:id="rId1"/>
-    <hyperlink ref="O6" location="StomaAnatomicalLocationCodelist!A1" display="StomaAnatomicalLocationCodelist"/>
-    <hyperlink ref="O7" location="StomaLateralityCodelist!A1" display="StomaLateralityCodelist"/>
+    <hyperlink ref="O4" location="StomaTypeCodelist!A1" display="StomaTypeCodelist" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="O6" location="StomaAnatomicalLocationCodelist!A1" display="StomaAnatomicalLocationCodelist" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="O7" location="StomaLateralityCodelist!A1" display="StomaLateralityCodelist" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1263,7 +1264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>